<commit_message>
[Shubham] Updated code on 12-09-24
</commit_message>
<xml_diff>
--- a/data/excel/HotelManualBooking.xlsx
+++ b/data/excel/HotelManualBooking.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C6F3DF-733E-4AAD-9FCA-0A80F9956A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DAD4A2-1EA9-45E7-BC24-79B50D322320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
+    <sheet name="BODC" sheetId="3" r:id="rId3"/>
+    <sheet name="BOCA" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="137">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -343,18 +344,6 @@
     <t>Test MO 5</t>
   </si>
   <si>
-    <t>Verify manual booking for one way flight with 1 adult</t>
-  </si>
-  <si>
-    <t>k.gaurav</t>
-  </si>
-  <si>
-    <t>Gaurav@130</t>
-  </si>
-  <si>
-    <t>ankit@quadlabs.com</t>
-  </si>
-  <si>
     <t>HotelName</t>
   </si>
   <si>
@@ -428,13 +417,31 @@
   </si>
   <si>
     <t>Verify manual booking for hotel with 2 adult , 2 child and 1 infant</t>
+  </si>
+  <si>
+    <t>15-Sep-2024</t>
+  </si>
+  <si>
+    <t>17-Sep-2024</t>
+  </si>
+  <si>
+    <t>ankur_QL</t>
+  </si>
+  <si>
+    <t>Ankur@12345</t>
+  </si>
+  <si>
+    <t>piyush.chauhan@quadlabs.com</t>
+  </si>
+  <si>
+    <t>Ankush009@quadlabs.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,6 +468,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF555555"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -522,7 +535,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -533,7 +546,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1317,7 +1331,7 @@
   <dimension ref="A1:BL4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2214,8 +2228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D8A60BA-B3CF-40F5-BA52-FF2E931720C5}">
   <dimension ref="A1:AG6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="X11" sqref="X11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2226,8 +2240,8 @@
     <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
@@ -2304,52 +2318,52 @@
         <v>79</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="R1" s="6" t="s">
         <v>25</v>
       </c>
       <c r="S1" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="V1" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="X1" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y1" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="V1" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="W1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="X1" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="Z1" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>123</v>
       </c>
       <c r="AB1" s="6" t="s">
         <v>27</v>
       </c>
       <c r="AC1" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD1" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="AF1" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="AD1" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="AE1" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="AF1" s="6" t="s">
-        <v>128</v>
       </c>
       <c r="AG1" s="6" t="s">
         <v>41</v>
@@ -2360,7 +2374,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>8</v>
@@ -2372,13 +2386,13 @@
         <v>10</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>109</v>
+        <v>134</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="I2" s="9">
         <v>1</v>
@@ -2405,7 +2419,7 @@
         <v>84</v>
       </c>
       <c r="Q2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="R2" t="s">
         <v>26</v>
@@ -2414,25 +2428,25 @@
         <v>16</v>
       </c>
       <c r="T2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>65</v>
+        <v>131</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="W2" t="s">
         <v>24</v>
       </c>
       <c r="X2">
-        <v>9999999006</v>
+        <v>9999999101</v>
       </c>
       <c r="Y2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="Z2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AA2">
         <v>1</v>
@@ -2447,10 +2461,10 @@
         <v>3</v>
       </c>
       <c r="AE2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="AF2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="AG2" t="s">
         <v>42</v>
@@ -2461,7 +2475,7 @@
         <v>71</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>8</v>
@@ -2473,13 +2487,13 @@
         <v>10</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>109</v>
+        <v>134</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="I3" s="9">
         <v>1</v>
@@ -2506,7 +2520,7 @@
         <v>84</v>
       </c>
       <c r="Q3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
@@ -2515,25 +2529,25 @@
         <v>16</v>
       </c>
       <c r="T3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="U3" s="7" t="s">
-        <v>65</v>
+        <v>131</v>
       </c>
       <c r="V3" s="7" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="W3" t="s">
         <v>24</v>
       </c>
       <c r="X3">
-        <v>9999999007</v>
+        <v>9999999102</v>
       </c>
       <c r="Y3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="Z3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AA3">
         <v>1</v>
@@ -2548,10 +2562,10 @@
         <v>2</v>
       </c>
       <c r="AE3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="AF3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="AG3" t="s">
         <v>42</v>
@@ -2562,7 +2576,7 @@
         <v>103</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>8</v>
@@ -2574,13 +2588,13 @@
         <v>10</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>109</v>
+        <v>134</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="I4" s="9">
         <v>1</v>
@@ -2607,7 +2621,7 @@
         <v>84</v>
       </c>
       <c r="Q4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="R4" t="s">
         <v>26</v>
@@ -2616,25 +2630,25 @@
         <v>16</v>
       </c>
       <c r="T4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>65</v>
+        <v>131</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="W4" t="s">
         <v>24</v>
       </c>
       <c r="X4">
-        <v>9999999008</v>
+        <v>9999999103</v>
       </c>
       <c r="Y4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="Z4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AA4">
         <v>1</v>
@@ -2649,10 +2663,10 @@
         <v>3</v>
       </c>
       <c r="AE4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="AF4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="AG4" t="s">
         <v>42</v>
@@ -2663,7 +2677,7 @@
         <v>104</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>8</v>
@@ -2675,13 +2689,13 @@
         <v>10</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>109</v>
+        <v>134</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="I5" s="9">
         <v>2</v>
@@ -2708,7 +2722,7 @@
         <v>84</v>
       </c>
       <c r="Q5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="R5" t="s">
         <v>26</v>
@@ -2717,25 +2731,25 @@
         <v>16</v>
       </c>
       <c r="T5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>65</v>
+        <v>131</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="W5" t="s">
         <v>24</v>
       </c>
       <c r="X5">
-        <v>9999999009</v>
+        <v>9999999104</v>
       </c>
       <c r="Y5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="Z5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AA5">
         <v>1</v>
@@ -2750,10 +2764,10 @@
         <v>3</v>
       </c>
       <c r="AE5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="AF5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="AG5" t="s">
         <v>42</v>
@@ -2764,7 +2778,7 @@
         <v>105</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>8</v>
@@ -2776,13 +2790,13 @@
         <v>10</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>109</v>
+        <v>134</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="I6" s="9">
         <v>2</v>
@@ -2809,7 +2823,7 @@
         <v>84</v>
       </c>
       <c r="Q6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="R6" t="s">
         <v>26</v>
@@ -2818,25 +2832,25 @@
         <v>16</v>
       </c>
       <c r="T6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>65</v>
+        <v>131</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="W6" t="s">
         <v>24</v>
       </c>
       <c r="X6">
-        <v>9999999010</v>
+        <v>9999999105</v>
       </c>
       <c r="Y6" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="Z6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AA6">
         <v>1</v>
@@ -2851,10 +2865,10 @@
         <v>2</v>
       </c>
       <c r="AE6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="AF6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="AG6" t="s">
         <v>42</v>
@@ -2869,12 +2883,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6" xr:uid="{997C06AD-95DE-46E9-A103-AB8581E765AB}">
       <formula1>"at,qlabs12345"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F6" xr:uid="{0F5C1780-0960-471C-8CF0-9D2144C9A77E}">
-      <formula1>"Piyush_QL,k.gaurav"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G6" xr:uid="{EAE2826F-53AE-46A3-BEBA-3E124A03DCF8}">
-      <formula1>"Password@123456,Gaurav@130"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG2:AG6" xr:uid="{4688F7E0-FA8B-42FE-B338-8F1C12A449F6}">
       <formula1>"Adjustment,Bank Draft,Inter Booking Transfer,Net Banking,Credit Card,Bank Transfer,Debit Card,Cash,Cheque,Direct Deposit"</formula1>
     </dataValidation>
@@ -2890,43 +2898,47 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R6" xr:uid="{C4067F69-FA98-44CB-87CB-336EA4A31BDB}">
       <formula1>"ABC Supplier,ATsupplier,BSP Supplier,gaurav travel"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G6" xr:uid="{9D849E6D-0572-4BCD-A837-F48EDADCB178}">
+      <formula1>"Password@@12,Gaurav@130,Ankur@12345"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F6" xr:uid="{B301C82A-6DF7-42E7-A060-56B86DF17D94}">
+      <formula1>"Piyush_QL,k.gaurav,ankur_QL"</formula1>
+    </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="shubham.natkar@quadlabs.com" xr:uid="{3E59DFD6-1FBE-4DC0-BBB8-62E2CE361ED8}"/>
-    <hyperlink ref="G2" r:id="rId2" display="Piyush@321" xr:uid="{B75E25C0-195E-4B46-A3E1-F3E3E71DBED6}"/>
-    <hyperlink ref="H2" r:id="rId3" xr:uid="{3FE8A31E-A084-4D53-8AD6-6500A8D37DC7}"/>
-    <hyperlink ref="F3" r:id="rId4" display="shubham.natkar@quadlabs.com" xr:uid="{F4DCBC23-1EAA-4CBC-BEC8-43D9C0967333}"/>
-    <hyperlink ref="F4" r:id="rId5" display="shubham.natkar@quadlabs.com" xr:uid="{8D4D5A83-6EF1-46E3-9C8D-2E95355B045A}"/>
-    <hyperlink ref="F5" r:id="rId6" display="shubham.natkar@quadlabs.com" xr:uid="{22FBCD3E-21A0-43FB-8BAA-635B04F73DAE}"/>
-    <hyperlink ref="F6" r:id="rId7" display="shubham.natkar@quadlabs.com" xr:uid="{65FD283E-38CC-4E41-BE10-2E8D4E273101}"/>
-    <hyperlink ref="G3" r:id="rId8" display="Piyush@321" xr:uid="{41428C6E-5713-4D55-A0F1-1DFBDFE1031B}"/>
-    <hyperlink ref="G4" r:id="rId9" display="Piyush@321" xr:uid="{5A9B1097-E1B3-44A0-BD15-8E455252A79E}"/>
-    <hyperlink ref="G5" r:id="rId10" display="Piyush@321" xr:uid="{88BCA966-F3DA-4BCC-A78E-91B0F6E70667}"/>
-    <hyperlink ref="G6" r:id="rId11" display="Piyush@321" xr:uid="{068C6FA9-B1DB-404D-B318-CB35EE0E350F}"/>
-    <hyperlink ref="H3:H6" r:id="rId12" display="ankit@quadlabs.com" xr:uid="{FB8EB32E-D085-45BF-8E12-C55A24892B4E}"/>
+    <hyperlink ref="F2" r:id="rId1" display="shubham.natkar@quadlabs.com" xr:uid="{679E64FA-F7A4-440C-A770-18F6FB8E54B5}"/>
+    <hyperlink ref="G2" r:id="rId2" display="Piyush@321" xr:uid="{4F77F8A7-EE9B-40B7-B3DA-5979EEE3DE82}"/>
+    <hyperlink ref="F3" r:id="rId3" display="shubham.natkar@quadlabs.com" xr:uid="{4CF80D20-F189-4A66-8563-0EB18EDAC338}"/>
+    <hyperlink ref="G3" r:id="rId4" display="Piyush@321" xr:uid="{B86AB1E8-473B-4644-AAFB-B7E4BEFD16FD}"/>
+    <hyperlink ref="F4" r:id="rId5" display="shubham.natkar@quadlabs.com" xr:uid="{0A4AEE39-4DCD-4016-A91B-DFBC4F8DD768}"/>
+    <hyperlink ref="G4" r:id="rId6" display="Piyush@321" xr:uid="{5650DA51-EE5C-4079-BA99-C68A0DAD78B8}"/>
+    <hyperlink ref="F5" r:id="rId7" display="shubham.natkar@quadlabs.com" xr:uid="{FCD789AA-C3DC-4182-8219-C24B1E217E11}"/>
+    <hyperlink ref="G5" r:id="rId8" display="Piyush@321" xr:uid="{253CD65C-753E-4EF1-A5E9-9653E811E6C1}"/>
+    <hyperlink ref="F6" r:id="rId9" display="shubham.natkar@quadlabs.com" xr:uid="{DE904B68-71C6-448B-B113-15BB5E7AB969}"/>
+    <hyperlink ref="G6" r:id="rId10" display="Piyush@321" xr:uid="{9A34F604-6E9E-4C82-91D4-CE8462384A2F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D365445-9CE4-48C5-99D0-16DC38F27301}">
-  <dimension ref="A1:AG2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B4D273-3F24-48EC-BE03-C6C1573B7DF3}">
+  <dimension ref="A1:AG6"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:AG2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
@@ -2939,10 +2951,15 @@
     <col min="18" max="18" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="16.28515625" bestFit="1" customWidth="1"/>
@@ -2998,52 +3015,52 @@
         <v>79</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="R1" s="6" t="s">
         <v>25</v>
       </c>
       <c r="S1" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="V1" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="X1" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y1" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="V1" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="W1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="X1" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="Z1" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>123</v>
       </c>
       <c r="AB1" s="6" t="s">
         <v>27</v>
       </c>
       <c r="AC1" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD1" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="AF1" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="AD1" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="AE1" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="AF1" s="6" t="s">
-        <v>128</v>
       </c>
       <c r="AG1" s="6" t="s">
         <v>41</v>
@@ -3054,7 +3071,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>8</v>
@@ -3066,22 +3083,22 @@
         <v>10</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>109</v>
+        <v>133</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>135</v>
       </c>
       <c r="I2" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J2" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>80</v>
@@ -3099,7 +3116,7 @@
         <v>84</v>
       </c>
       <c r="Q2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="R2" t="s">
         <v>26</v>
@@ -3108,25 +3125,25 @@
         <v>16</v>
       </c>
       <c r="T2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>65</v>
+        <v>131</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="W2" t="s">
         <v>24</v>
       </c>
       <c r="X2">
-        <v>9999999990</v>
+        <v>9999999101</v>
       </c>
       <c r="Y2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="Z2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AA2">
         <v>1</v>
@@ -3141,49 +3158,716 @@
         <v>3</v>
       </c>
       <c r="AE2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="I3" s="9">
+        <v>1</v>
+      </c>
+      <c r="J3" s="9">
+        <v>1</v>
+      </c>
+      <c r="K3" s="9">
+        <v>0</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="M3" t="s">
+        <v>81</v>
+      </c>
+      <c r="N3" t="s">
+        <v>82</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>107</v>
+      </c>
+      <c r="R3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T3" t="s">
+        <v>110</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="W3" t="s">
+        <v>24</v>
+      </c>
+      <c r="X3">
+        <v>9999999102</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>10</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD3" s="9">
+        <v>2</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>123</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>125</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="I4" s="9">
+        <v>1</v>
+      </c>
+      <c r="J4" s="9">
+        <v>1</v>
+      </c>
+      <c r="K4" s="9">
+        <v>1</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="M4" t="s">
+        <v>81</v>
+      </c>
+      <c r="N4" t="s">
+        <v>82</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>107</v>
+      </c>
+      <c r="R4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S4" t="s">
+        <v>16</v>
+      </c>
+      <c r="T4" t="s">
+        <v>110</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="W4" t="s">
+        <v>24</v>
+      </c>
+      <c r="X4">
+        <v>9999999103</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA4">
+        <v>1</v>
+      </c>
+      <c r="AB4">
+        <v>10</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD4" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>123</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>125</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="I5" s="9">
+        <v>2</v>
+      </c>
+      <c r="J5" s="9">
+        <v>1</v>
+      </c>
+      <c r="K5" s="9">
+        <v>1</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="M5" t="s">
+        <v>81</v>
+      </c>
+      <c r="N5" t="s">
+        <v>82</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>107</v>
+      </c>
+      <c r="R5" t="s">
+        <v>26</v>
+      </c>
+      <c r="S5" t="s">
+        <v>16</v>
+      </c>
+      <c r="T5" t="s">
+        <v>110</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="V5" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="W5" t="s">
+        <v>24</v>
+      </c>
+      <c r="X5">
+        <v>9999999104</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
+        <v>10</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD5" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>123</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>125</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="I6" s="9">
+        <v>2</v>
+      </c>
+      <c r="J6" s="9">
+        <v>2</v>
+      </c>
+      <c r="K6" s="9">
+        <v>1</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="M6" t="s">
+        <v>81</v>
+      </c>
+      <c r="N6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>107</v>
+      </c>
+      <c r="R6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S6" t="s">
+        <v>16</v>
+      </c>
+      <c r="T6" t="s">
+        <v>110</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="V6" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="W6" t="s">
+        <v>24</v>
+      </c>
+      <c r="X6">
+        <v>9999999105</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <v>10</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD6" s="9">
+        <v>2</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>123</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>125</v>
+      </c>
+      <c r="AG6" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="9">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{FEE6C5F7-DA33-4E50-BED6-8B9358E07870}">
-      <formula1>"Password@123456,Gaurav@130"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{CA2411DC-A4B9-4A30-B4DD-0A183CCCB139}">
-      <formula1>"Piyush_QL,k.gaurav"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{B6ED9948-B27F-42AD-A864-0F0D7583468C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F6" xr:uid="{12B42C73-F999-4F51-A5F2-8492B7B9A41B}">
+      <formula1>"Piyush_QL,k.gaurav,ankur_QL"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G6" xr:uid="{76F82B04-7C49-4317-B0F7-B63201651B77}">
+      <formula1>"Password@@12,Gaurav@130,Ankur@12345"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R6" xr:uid="{A9FE6039-10BA-4020-8017-488C8F8D5361}">
+      <formula1>"ABC Supplier,ATsupplier,BSP Supplier,gaurav travel"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2:W6" xr:uid="{7D7ABD5A-8E8C-4803-A433-9817023026AA}">
+      <formula1>"HK,RQ"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2:AD6" xr:uid="{A7785F74-16D8-4C07-ACE8-E36FB4DB58A4}">
+      <formula1>"1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2:AC6" xr:uid="{47D8A0AD-9DC8-4068-A128-2481F9A418DB}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG2:AG6" xr:uid="{915F38AF-0A93-4303-8E6E-214538F23E08}">
+      <formula1>"Adjustment,Bank Draft,Inter Booking Transfer,Net Banking,Credit Card,Bank Transfer,Debit Card,Cash,Cheque,Direct Deposit"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6" xr:uid="{96E2FD96-6051-4ADB-85FE-5A8E16B10125}">
       <formula1>"at,qlabs12345"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:K2" xr:uid="{BFE0DFBC-7B79-4D7E-BD22-870B6E00C8F3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:K6" xr:uid="{84E6A7BF-58DE-4029-9A67-087119EB4C6E}">
       <formula1>"0,1,2,3,4,5"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2" xr:uid="{D0C9C227-F091-44CC-A792-ECDD2525C192}">
-      <formula1>"ABC Supplier,ATsupplier,BSP Supplier,gaurav travel"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2" xr:uid="{5A84A3CB-36FD-4F53-B8E5-B961BE37E4E1}">
-      <formula1>"HK,RQ"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2" xr:uid="{0583031B-4236-464D-8715-A76A8B502D0D}">
-      <formula1>"1,2,3,4,5"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2" xr:uid="{B2F95911-9C1F-4A45-A4F9-FDADE3FB3142}">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG2" xr:uid="{F86F5309-D358-463F-BAE0-38E90CF7B233}">
-      <formula1>"Adjustment,Bank Draft,Inter Booking Transfer,Net Banking,Credit Card,Bank Transfer,Debit Card,Cash,Cheque,Direct Deposit"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="shubham.natkar@quadlabs.com" xr:uid="{38772896-79D0-4FF5-9B3F-EEC51EA1C0D3}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{00FDBF7A-1845-4F55-99CB-177ACEFEB8C2}"/>
-    <hyperlink ref="H2" r:id="rId3" xr:uid="{F98F79F7-4E4F-4118-B2C2-B4349A916B62}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{9BF333CB-06D9-4CD9-A242-681928621E30}"/>
+    <hyperlink ref="F2" r:id="rId2" display="shubham.natkar@quadlabs.com" xr:uid="{2CCE7BD8-9BB0-45E2-A823-AFF1D33CC2A5}"/>
+    <hyperlink ref="G2" r:id="rId3" display="Piyush@321" xr:uid="{DDDE4D97-11E3-4AD7-8DD4-34690AAA35FC}"/>
+    <hyperlink ref="H3" r:id="rId4" xr:uid="{A10D9730-0765-4FFD-9F1E-2FDDE972423C}"/>
+    <hyperlink ref="F3" r:id="rId5" display="shubham.natkar@quadlabs.com" xr:uid="{D82FECC6-E3E9-45D7-9752-7FCF850CC8A7}"/>
+    <hyperlink ref="G3" r:id="rId6" display="Piyush@321" xr:uid="{531CB571-1D72-458F-A4DE-6B3B986D17F0}"/>
+    <hyperlink ref="H4" r:id="rId7" xr:uid="{4EF6CE67-E6E5-4380-AEE2-C5AD6CAE193F}"/>
+    <hyperlink ref="F4" r:id="rId8" display="shubham.natkar@quadlabs.com" xr:uid="{358573E9-D6B7-4EEE-9666-5D42A57C59A4}"/>
+    <hyperlink ref="G4" r:id="rId9" display="Piyush@321" xr:uid="{215C5B1C-A192-4DFC-A1FD-13772550D649}"/>
+    <hyperlink ref="H5" r:id="rId10" xr:uid="{C7952641-26B6-4BD2-BDD3-AEE62CDEAB6B}"/>
+    <hyperlink ref="F5" r:id="rId11" display="shubham.natkar@quadlabs.com" xr:uid="{D4B9C271-419A-492A-8244-219371F6522F}"/>
+    <hyperlink ref="G5" r:id="rId12" display="Piyush@321" xr:uid="{F0145A6E-806E-4229-87DD-7D372F933177}"/>
+    <hyperlink ref="H6" r:id="rId13" xr:uid="{4FB57809-29F5-4CF6-AC75-8FC184D4CABB}"/>
+    <hyperlink ref="F6" r:id="rId14" display="shubham.natkar@quadlabs.com" xr:uid="{589CFEC6-0EF5-436B-833E-B9E1D1CA5366}"/>
+    <hyperlink ref="G6" r:id="rId15" display="Piyush@321" xr:uid="{0E19E1E4-7B94-41CC-8BEC-1F46E7F76F53}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED204D34-4B38-4CE6-B3A2-9F55432253BD}">
+  <dimension ref="A1:AG2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD1" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="AF1" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="AG1" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="I2" s="9">
+        <v>2</v>
+      </c>
+      <c r="J2" s="9">
+        <v>1</v>
+      </c>
+      <c r="K2" s="9">
+        <v>1</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="M2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>107</v>
+      </c>
+      <c r="R2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" t="s">
+        <v>110</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="W2" t="s">
+        <v>24</v>
+      </c>
+      <c r="X2">
+        <v>9999999104</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>10</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD2" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:K2" xr:uid="{7E8A2F59-D96B-45A0-82CD-ED332EA05DB5}">
+      <formula1>"0,1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{ECA8E870-E511-4CF7-A454-5C075A82DB6A}">
+      <formula1>"at,qlabs12345"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG2" xr:uid="{4BEB42D1-92A3-412B-BB52-04798C7EF036}">
+      <formula1>"Adjustment,Bank Draft,Inter Booking Transfer,Net Banking,Credit Card,Bank Transfer,Debit Card,Cash,Cheque,Direct Deposit"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2" xr:uid="{F75C5611-67EA-46A2-BA00-D17920027D2A}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2" xr:uid="{51DBC8A7-7130-4B3D-B204-FA72A8C479D2}">
+      <formula1>"1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2" xr:uid="{8DA60AD8-7076-451E-89E5-B8FFCAFBB625}">
+      <formula1>"HK,RQ"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2" xr:uid="{2F693E2F-7A76-4AB0-9978-694775DE9563}">
+      <formula1>"ABC Supplier,ATsupplier,BSP Supplier,gaurav travel"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{37846A5E-6F6C-4698-A9D9-EB04DC0D1DAF}">
+      <formula1>"Password@@12,Gaurav@130,Ankur@12345"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{59128AF9-1725-4E6A-AC6E-A00675242851}">
+      <formula1>"Piyush_QL,k.gaurav,ankur_QL"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{3FDBDC7E-63BF-4BA4-BA4A-9D82256C860C}"/>
+    <hyperlink ref="F2" r:id="rId2" display="shubham.natkar@quadlabs.com" xr:uid="{4DCAF0A5-83DA-4426-888B-62D3EBA11B94}"/>
+    <hyperlink ref="G2" r:id="rId3" display="Piyush@321" xr:uid="{3C17E4EA-4F38-419F-B8D4-FB2665F96650}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>